<commit_message>
re-ran parsing routines and corrected example data
</commit_message>
<xml_diff>
--- a/docs/files/isotherm.xlsx
+++ b/docs/files/isotherm.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="92DEC378012DEF26EC64FB0A16AB70C9F6AB99A3" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{B196EAA9-CADE-432D-8A11-51E211D041B6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56911A87-80BA-43B8-904A-2FD4E992C805}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,84 +15,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>(en °C)</t>
-  </si>
-  <si>
-    <t>(en K)</t>
-  </si>
-  <si>
-    <t>Pressure(bar)</t>
-  </si>
-  <si>
-    <t>Enthalpy(kJ/mol)</t>
-  </si>
-  <si>
-    <t>Calorimetrie</t>
-  </si>
-  <si>
-    <t>Type manip</t>
-  </si>
-  <si>
-    <t>Experience ou Simulation</t>
-  </si>
-  <si>
-    <t>Date de l'expérience</t>
-  </si>
-  <si>
-    <t>Nom de l'échantillon</t>
-  </si>
-  <si>
-    <t>Lot de l'échantillon</t>
-  </si>
-  <si>
-    <t>Température d'activation (°C)</t>
-  </si>
-  <si>
-    <t>Surnom de l'appareil</t>
-  </si>
-  <si>
-    <t>Température de l'expérience (K)</t>
-  </si>
-  <si>
-    <t>Formule chimique du gaz</t>
-  </si>
-  <si>
-    <t>Surnom du contact</t>
-  </si>
-  <si>
-    <t>Nom du projet</t>
-  </si>
-  <si>
-    <t>Experience</t>
-  </si>
-  <si>
-    <t>ADW</t>
-  </si>
-  <si>
-    <t>EU MACADEMIA</t>
-  </si>
-  <si>
-    <t>KRICT</t>
-  </si>
-  <si>
-    <t>CV</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>CO2</t>
   </si>
   <si>
-    <t>Nom du labo</t>
-  </si>
-  <si>
-    <t>MADIREL</t>
-  </si>
-  <si>
     <t>HKUST-1(Cu)</t>
   </si>
   <si>
-    <t>Loading(mmol/g)</t>
+    <t>Sample name</t>
+  </si>
+  <si>
+    <t>Sample batch</t>
+  </si>
+  <si>
+    <t>Experiment temperature (K)</t>
+  </si>
+  <si>
+    <t>Adsorbate used</t>
+  </si>
+  <si>
+    <t>Pressure mode</t>
+  </si>
+  <si>
+    <t>Pressure unit</t>
+  </si>
+  <si>
+    <t>Loading basis</t>
+  </si>
+  <si>
+    <t>Loading unit</t>
+  </si>
+  <si>
+    <t>Adsorbent basis</t>
+  </si>
+  <si>
+    <t>Adsorbent unit</t>
+  </si>
+  <si>
+    <t>Isotherm data</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>loading</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>molar</t>
+  </si>
+  <si>
+    <t>mmol</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>enthalpy(kJ/mol)</t>
   </si>
 </sst>
 </file>
@@ -104,7 +95,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,21 +112,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +131,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,11 +141,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -187,50 +159,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,491 +529,471 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>303</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
-        <v>40319</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
-        <v>150</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6">
-        <v>303</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="6">
         <v>0.15583870967741936</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B13" s="6">
         <v>0.76232823703504282</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C13" s="7">
         <v>28.787968605148585</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="6">
         <v>0.32593870967741939</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B14" s="6">
         <v>1.5333490038558755</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C14" s="7">
         <v>28.76093926373845</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="6">
         <v>0.55443870967741937</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B15" s="6">
         <v>2.4975726550081814</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C15" s="7">
         <v>28.749976751048372</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="6">
         <v>0.80723870967741929</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B16" s="6">
         <v>3.4701210328210239</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C16" s="7">
         <v>28.848169714242211</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="6">
         <v>1.0339387096774195</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B17" s="6">
         <v>4.2555060735869281</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C17" s="7">
         <v>28.962935200001663</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="6">
         <v>1.2515387096774195</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B18" s="6">
         <v>4.9353678051874921</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C18" s="7">
         <v>28.848868914480789</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="6">
         <v>1.5303387096774195</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B19" s="6">
         <v>5.7125732076499176</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C19" s="7">
         <v>28.736356320940175</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="6">
         <v>1.8097387096774193</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B20" s="6">
         <v>6.3970077640295617</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C20" s="7">
         <v>28.576630998935098</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="6">
         <v>2.0767387096774192</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B21" s="6">
         <v>6.9738998777425749</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C21" s="7">
         <v>28.536650328193513</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="6">
         <v>3.4574387096774193</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B22" s="6">
         <v>9.1217399944396984</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C22" s="7">
         <v>28.970042713971647</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="6">
         <v>5.361338709677419</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B23" s="6">
         <v>10.796429857290937</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C23" s="7">
         <v>29.791154046048455</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="6">
         <v>6.7474387096774189</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B24" s="6">
         <v>11.526439080096157</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C24" s="7">
         <v>31.492626288961134</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="6">
         <v>9.1746387096774189</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B25" s="6">
         <v>12.356451494044723</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C25" s="7">
         <v>32.981036399153666</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="6">
         <v>10.660938709677419</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B26" s="6">
         <v>12.657298507214398</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C26" s="7">
         <v>39.655295151492183</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="6">
         <v>12.10943870967742</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B27" s="6">
         <v>12.931024479600852</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C27" s="7">
         <v>35.165581329247829</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="6">
         <v>15.141638709677419</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B28" s="6">
         <v>13.471568862314383</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C28" s="7">
         <v>30.487290433683537</v>
       </c>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="6">
         <v>16.873838709677418</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B29" s="6">
         <v>13.778726163000288</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C29" s="7">
         <v>25.011149294774494</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="6">
         <v>18.41893870967742</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B30" s="6">
         <v>14.059022287512292</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C30" s="7">
         <v>22.062288826305295</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="6">
         <v>20.187638709677419</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B31" s="6">
         <v>14.386412050686149</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C31" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="6">
         <v>24.67963870967742</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B32" s="6">
         <v>15.003115149028487</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C32" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="6">
         <v>22.197238709677418</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B33" s="6">
         <v>14.938013754923421</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C33" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="6">
         <v>18.271538709677419</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B34" s="6">
         <v>14.713636962167575</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C34" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="6">
         <v>14.97453870967742</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B35" s="6">
         <v>14.404348311679856</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C35" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="6">
         <v>12.235538709677419</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B36" s="6">
         <v>14.023376995875864</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C36" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="6">
         <v>9.3094387096774192</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B37" s="6">
         <v>13.403952042340714</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C37" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="6">
         <v>6.7259387096774192</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B38" s="6">
         <v>12.531108583675916</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C38" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="6">
         <v>4.4989387096774189</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B39" s="6">
         <v>11.199293306973249</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C39" s="7">
         <v>20.185751891058665</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="14"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="14"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="14"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="14"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="14"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="14"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>